<commit_message>
Archivo para importar usuarios
</commit_message>
<xml_diff>
--- a/Usuarios ejemplo.xlsx
+++ b/Usuarios ejemplo.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\proyecto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8CACA70-1C5D-4485-B961-A4B522BBD0F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{214E4197-A47A-4C29-82A3-B9A650A37A4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{C220839A-B43B-4147-8C15-1B1F48ECE72D}"/>
   </bookViews>
   <sheets>
     <sheet name="militantes" sheetId="8" r:id="rId1"/>
+    <sheet name="Hoja1" sheetId="9" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">militantes!$A$3:$E$3</definedName>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="69">
   <si>
     <t>Username</t>
   </si>
@@ -261,6 +262,9 @@
   </si>
   <si>
     <t>',first_name='</t>
+  </si>
+  <si>
+    <t>usuario = Militante.objects.update(username='70000',first_name='john',last_name='john', email='sistemas@partidoverde.org.co', password='70000', is_active= False, location= puesto )</t>
   </si>
 </sst>
 </file>
@@ -654,7 +658,7 @@
   <dimension ref="A1:M33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -707,7 +711,7 @@
         <v>56</v>
       </c>
       <c r="E4" t="str">
-        <f>D4</f>
+        <f t="shared" ref="E4:E26" si="0">D4</f>
         <v>Catalina castiblanco</v>
       </c>
       <c r="F4" t="s">
@@ -748,11 +752,11 @@
         <v>18</v>
       </c>
       <c r="E5" t="str">
-        <f>D5</f>
+        <f t="shared" si="0"/>
         <v>Jurani</v>
       </c>
       <c r="M5" s="5" t="str">
-        <f t="shared" ref="M5:M26" si="0">CONCATENATE($F$4,A5,$G$4,D5,$H$4,E5,$I$4,B5,$J$4,A5,$K$4)</f>
+        <f t="shared" ref="M5:M28" si="1">CONCATENATE($F$4,A5,$G$4,D5,$H$4,E5,$I$4,B5,$J$4,A5,$K$4)</f>
         <v>usuario = Militante.objects.create_user(username='120000',first_name='Jurani',last_name='Jurani', email='asistentecontable@partidoverde.org.co', password='120000', is_active= False, location= puesto )</v>
       </c>
     </row>
@@ -770,11 +774,11 @@
         <v>13</v>
       </c>
       <c r="E6" t="str">
-        <f>D6</f>
+        <f t="shared" si="0"/>
         <v>Wendi</v>
       </c>
       <c r="M6" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>usuario = Militante.objects.create_user(username='80000',first_name='Wendi',last_name='Wendi', email='asosoriajuridica1@partidoverde.org.co', password='80000', is_active= False, location= puesto )</v>
       </c>
     </row>
@@ -792,11 +796,11 @@
         <v>8</v>
       </c>
       <c r="E7" t="str">
-        <f>D7</f>
+        <f t="shared" si="0"/>
         <v>Carlos</v>
       </c>
       <c r="M7" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>usuario = Militante.objects.create_user(username='30000',first_name='Carlos',last_name='Carlos', email='audiovisuales@alianzaverde.org.co', password='30000', is_active= False, location= puesto )</v>
       </c>
     </row>
@@ -814,11 +818,11 @@
         <v>20</v>
       </c>
       <c r="E8" t="str">
-        <f>D8</f>
+        <f t="shared" si="0"/>
         <v>Angela</v>
       </c>
       <c r="M8" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>usuario = Militante.objects.create_user(username='130000',first_name='Angela',last_name='Angela', email='auditoria-angela@partidoverde.org.co', password='130000', is_active= False, location= puesto )</v>
       </c>
     </row>
@@ -836,11 +840,11 @@
         <v>21</v>
       </c>
       <c r="E9" t="str">
-        <f>D9</f>
+        <f t="shared" si="0"/>
         <v>Carmen</v>
       </c>
       <c r="M9" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>usuario = Militante.objects.create_user(username='140000',first_name='Carmen',last_name='Carmen', email='auditoria-carmen@partidoverde.org.co', password='140000', is_active= False, location= puesto )</v>
       </c>
     </row>
@@ -855,11 +859,11 @@
         <v>59</v>
       </c>
       <c r="E10" t="str">
-        <f>D10</f>
+        <f t="shared" si="0"/>
         <v>Lina quevedo</v>
       </c>
       <c r="M10" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>usuario = Militante.objects.create_user(username='230000',first_name='Lina quevedo',last_name='Lina quevedo', email='centropensammiento@partidoverde.org.co', password='230000', is_active= False, location= puesto )</v>
       </c>
     </row>
@@ -877,11 +881,11 @@
         <v>6</v>
       </c>
       <c r="E11" t="str">
-        <f>D11</f>
+        <f t="shared" si="0"/>
         <v>Monica</v>
       </c>
       <c r="M11" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>usuario = Militante.objects.create_user(username='10000',first_name='Monica',last_name='Monica', email='community@partidoverde.org.co', password='10000', is_active= False, location= puesto )</v>
       </c>
     </row>
@@ -899,11 +903,11 @@
         <v>16</v>
       </c>
       <c r="E12" t="str">
-        <f>D12</f>
+        <f t="shared" si="0"/>
         <v>Erika</v>
       </c>
       <c r="M12" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>usuario = Militante.objects.create_user(username='100000',first_name='Erika',last_name='Erika', email='contabilidad@partidoverde.org.co', password='100000', is_active= False, location= puesto )</v>
       </c>
     </row>
@@ -921,11 +925,11 @@
         <v>24</v>
       </c>
       <c r="E13" t="str">
-        <f>D13</f>
+        <f t="shared" si="0"/>
         <v>Valentina</v>
       </c>
       <c r="M13" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>usuario = Militante.objects.create_user(username='160000',first_name='Valentina',last_name='Valentina', email='cuentas13@partidoverde.org.co', password='160000', is_active= False, location= puesto )</v>
       </c>
     </row>
@@ -943,11 +947,11 @@
         <v>25</v>
       </c>
       <c r="E14" t="str">
-        <f>D14</f>
+        <f t="shared" si="0"/>
         <v>Vanesa</v>
       </c>
       <c r="M14" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>usuario = Militante.objects.create_user(username='180000',first_name='Vanesa',last_name='Vanesa', email='cuentas23@partidoverde.org.co', password='180000', is_active= False, location= puesto )</v>
       </c>
     </row>
@@ -965,11 +969,11 @@
         <v>45</v>
       </c>
       <c r="E15" t="str">
-        <f>D15</f>
+        <f t="shared" si="0"/>
         <v>GABRIELA JIMENEZ AGUIAR</v>
       </c>
       <c r="M15" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>usuario = Militante.objects.create_user(username='170000',first_name='GABRIELA JIMENEZ AGUIAR',last_name='GABRIELA JIMENEZ AGUIAR', email='cuentas25@partidoverde.org.co', password='170000', is_active= False, location= puesto )</v>
       </c>
     </row>
@@ -987,11 +991,11 @@
         <v>14</v>
       </c>
       <c r="E16" t="str">
-        <f>D16</f>
+        <f t="shared" si="0"/>
         <v>Alejandra</v>
       </c>
       <c r="M16" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>usuario = Militante.objects.create_user(username='90000',first_name='Alejandra',last_name='Alejandra', email='cuentas5@partidoverde.org.co', password='90000', is_active= False, location= puesto )</v>
       </c>
     </row>
@@ -1009,14 +1013,14 @@
         <v>23</v>
       </c>
       <c r="E17" t="str">
-        <f>D17</f>
+        <f t="shared" si="0"/>
         <v>Wilches</v>
       </c>
       <c r="F17" t="s">
         <v>22</v>
       </c>
       <c r="M17" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>usuario = Militante.objects.create_user(username='150000',first_name='Wilches',last_name='Wilches', email='cuentas6@partidoverde.org.co', password='150000', is_active= False, location= puesto )</v>
       </c>
     </row>
@@ -1034,11 +1038,11 @@
         <v>9</v>
       </c>
       <c r="E18" t="str">
-        <f>D18</f>
+        <f t="shared" si="0"/>
         <v>Daniel</v>
       </c>
       <c r="M18" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>usuario = Militante.objects.create_user(username='50000',first_name='Daniel',last_name='Daniel', email='desarollotecnologico@partidoverde.org.co', password='50000', is_active= False, location= puesto )</v>
       </c>
     </row>
@@ -1056,11 +1060,11 @@
         <v>7</v>
       </c>
       <c r="E19" t="str">
-        <f>D19</f>
+        <f t="shared" si="0"/>
         <v>Natali</v>
       </c>
       <c r="M19" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>usuario = Militante.objects.create_user(username='20000',first_name='Natali',last_name='Natali', email='diseno@partidoverde.org.co', password='20000', is_active= False, location= puesto )</v>
       </c>
     </row>
@@ -1078,11 +1082,11 @@
         <v>10</v>
       </c>
       <c r="E20" t="str">
-        <f>D20</f>
+        <f t="shared" si="0"/>
         <v>Diego</v>
       </c>
       <c r="M20" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>usuario = Militante.objects.create_user(username='60000',first_name='Diego',last_name='Diego', email='dzambrano@partidoverde.org.co', password='60000', is_active= False, location= puesto )</v>
       </c>
     </row>
@@ -1097,11 +1101,11 @@
         <v>57</v>
       </c>
       <c r="E21" t="str">
-        <f>D21</f>
+        <f t="shared" si="0"/>
         <v>Laura vasquez</v>
       </c>
       <c r="M21" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>usuario = Militante.objects.create_user(username='210000',first_name='Laura vasquez',last_name='Laura vasquez', email='escueladegobierno@partidoverde.org.co', password='210000', is_active= False, location= puesto )</v>
       </c>
     </row>
@@ -1119,11 +1123,11 @@
         <v>17</v>
       </c>
       <c r="E22" t="str">
-        <f>D22</f>
+        <f t="shared" si="0"/>
         <v>Lina</v>
       </c>
       <c r="M22" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>usuario = Militante.objects.create_user(username='110000',first_name='Lina',last_name='Lina', email='pagos@partidoverde.org.co', password='110000', is_active= False, location= puesto )</v>
       </c>
     </row>
@@ -1141,11 +1145,11 @@
         <v>46</v>
       </c>
       <c r="E23" t="str">
-        <f>D23</f>
+        <f t="shared" si="0"/>
         <v xml:space="preserve">Andres Felipe Gil Lozano </v>
       </c>
       <c r="M23" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>usuario = Militante.objects.create_user(username='40000',first_name='Andres Felipe Gil Lozano ',last_name='Andres Felipe Gil Lozano ', email='realizador@partidoverde.org.co', password='40000', is_active= False, location= puesto )</v>
       </c>
     </row>
@@ -1163,11 +1167,11 @@
         <v>26</v>
       </c>
       <c r="E24" t="str">
-        <f>D24</f>
+        <f t="shared" si="0"/>
         <v>Dalia</v>
       </c>
       <c r="M24" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>usuario = Militante.objects.create_user(username='190000',first_name='Dalia',last_name='Dalia', email='recepcion@partidoverde.org.co', password='190000', is_active= False, location= puesto )</v>
       </c>
     </row>
@@ -1182,11 +1186,11 @@
         <v>58</v>
       </c>
       <c r="E25" t="str">
-        <f>D25</f>
+        <f t="shared" si="0"/>
         <v>Karol rojas</v>
       </c>
       <c r="M25" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>usuario = Militante.objects.create_user(username='220000',first_name='Karol rojas',last_name='Karol rojas', email='regiones@partidoverde.org.co', password='220000', is_active= False, location= puesto )</v>
       </c>
     </row>
@@ -1204,16 +1208,17 @@
         <v>11</v>
       </c>
       <c r="E26" t="str">
-        <f>D26</f>
+        <f t="shared" si="0"/>
         <v>john</v>
       </c>
       <c r="M26" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>usuario = Militante.objects.create_user(username='70000',first_name='john',last_name='john', email='sistemas@partidoverde.org.co', password='70000', is_active= False, location= puesto )</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B28" s="2"/>
+      <c r="M28" s="5"/>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B29" s="2"/>
@@ -1255,4 +1260,22 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId15"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F369B89-947C-4F5A-BC6E-EDC0E5C4AB4F}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>68</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>